<commit_message>
Rest of the MUSE points added
</commit_message>
<xml_diff>
--- a/CodeKernel_Manual_Data/MUSE Data/labels_muse.xlsx
+++ b/CodeKernel_Manual_Data/MUSE Data/labels_muse.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD781E9A-2A71-4CFE-90EB-F60112A86502}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FA17E4-7C34-4A9D-9160-8F1505E57786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1039,7 +1039,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1070,6 +1070,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -1083,7 +1101,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1099,11 +1117,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1445,14 +1469,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L121"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A75" sqref="A75:A82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="29.6640625" customWidth="1"/>
-    <col min="2" max="2" width="52.44140625" customWidth="1"/>
+    <col min="2" max="2" width="68.6640625" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="7" max="8" width="9.109375" customWidth="1"/>
     <col min="9" max="9" width="56.109375" style="6" customWidth="1"/>
@@ -1489,7 +1514,7 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="9" t="s">
+      <c r="A2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -1518,7 +1543,7 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="9"/>
+      <c r="A3" s="14"/>
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -1545,14 +1570,14 @@
       </c>
     </row>
     <row r="4" spans="1:9" ht="28.8">
-      <c r="A4" s="9"/>
-      <c r="B4" t="s">
+      <c r="A4" s="14"/>
+      <c r="B4" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="12">
         <v>0</v>
       </c>
       <c r="E4">
@@ -1572,14 +1597,14 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="28.8">
-      <c r="A5" s="9"/>
-      <c r="B5" t="s">
+      <c r="A5" s="14"/>
+      <c r="B5" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="12">
         <v>1</v>
       </c>
       <c r="E5">
@@ -1596,7 +1621,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" ht="43.2">
-      <c r="A6" s="9"/>
+      <c r="A6" s="14"/>
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -1623,7 +1648,7 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="9"/>
+      <c r="A7" s="14"/>
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -1650,14 +1675,14 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="9"/>
+      <c r="A8" s="14"/>
       <c r="B8" t="s">
         <v>19</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="12">
         <v>1</v>
       </c>
       <c r="E8">
@@ -1674,14 +1699,14 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="9"/>
+      <c r="A9" s="14"/>
       <c r="B9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="12">
         <v>3</v>
       </c>
       <c r="E9">
@@ -1701,7 +1726,7 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="9"/>
+      <c r="A10" s="14"/>
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -1725,7 +1750,7 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="9"/>
+      <c r="A11" s="14"/>
       <c r="B11" t="s">
         <v>22</v>
       </c>
@@ -1749,7 +1774,7 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="9"/>
+      <c r="A12" s="14"/>
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -1773,14 +1798,14 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="9"/>
+      <c r="A13" s="14"/>
       <c r="B13" t="s">
         <v>25</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="12">
         <v>2</v>
       </c>
       <c r="E13">
@@ -1797,9 +1822,9 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="9"/>
-      <c r="B14" s="9"/>
-      <c r="C14" s="9"/>
+      <c r="A14" s="11"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
       <c r="D14" s="2" t="s">
         <v>206</v>
       </c>
@@ -1811,7 +1836,7 @@
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="9" t="s">
+      <c r="A15" s="14" t="s">
         <v>28</v>
       </c>
       <c r="B15" t="s">
@@ -1840,14 +1865,14 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="9"/>
-      <c r="B16" t="s">
+      <c r="A16" s="14"/>
+      <c r="B16" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D16">
+      <c r="D16" s="12">
         <v>0</v>
       </c>
       <c r="E16">
@@ -1864,7 +1889,7 @@
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="9"/>
+      <c r="A17" s="14"/>
       <c r="B17" t="s">
         <v>31</v>
       </c>
@@ -1891,7 +1916,7 @@
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="9"/>
+      <c r="A18" s="14"/>
       <c r="B18" t="s">
         <v>33</v>
       </c>
@@ -1918,7 +1943,7 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="9"/>
+      <c r="A19" s="14"/>
       <c r="B19" t="s">
         <v>35</v>
       </c>
@@ -1942,14 +1967,14 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="9"/>
+      <c r="A20" s="14"/>
       <c r="B20" t="s">
         <v>36</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D20">
+      <c r="D20" s="12">
         <v>1</v>
       </c>
       <c r="E20">
@@ -1969,14 +1994,14 @@
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="9"/>
+      <c r="A21" s="14"/>
       <c r="B21" t="s">
         <v>38</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D21">
+      <c r="D21" s="12">
         <v>4</v>
       </c>
       <c r="E21">
@@ -1996,7 +2021,7 @@
       </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="9"/>
+      <c r="A22" s="14"/>
       <c r="B22" t="s">
         <v>40</v>
       </c>
@@ -2015,14 +2040,14 @@
       <c r="H22">
         <v>2</v>
       </c>
-      <c r="I22" s="10" t="s">
+      <c r="I22" s="9" t="s">
         <v>70</v>
       </c>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="9"/>
+      <c r="A23" s="14"/>
       <c r="B23" t="s">
         <v>42</v>
       </c>
@@ -2049,7 +2074,7 @@
       </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="9"/>
+      <c r="A24" s="14"/>
       <c r="B24" t="s">
         <v>44</v>
       </c>
@@ -2073,14 +2098,14 @@
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="9"/>
+      <c r="A25" s="14"/>
       <c r="B25" t="s">
         <v>45</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D25">
+      <c r="D25" s="12">
         <v>1</v>
       </c>
       <c r="E25">
@@ -2097,14 +2122,14 @@
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="9"/>
-      <c r="B26" t="s">
+      <c r="A26" s="14"/>
+      <c r="B26" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D26">
+      <c r="D26" s="12">
         <v>1</v>
       </c>
       <c r="E26">
@@ -2121,14 +2146,14 @@
       </c>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="9"/>
+      <c r="A27" s="14"/>
       <c r="B27" t="s">
         <v>168</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D27">
+      <c r="D27" s="12">
         <v>0</v>
       </c>
       <c r="E27">
@@ -2145,14 +2170,14 @@
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="9"/>
+      <c r="A28" s="14"/>
       <c r="B28" t="s">
         <v>46</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D28">
+      <c r="D28" s="12">
         <v>1</v>
       </c>
       <c r="E28">
@@ -2174,14 +2199,14 @@
       <c r="K28" s="4"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="9"/>
+      <c r="A29" s="14"/>
       <c r="B29" t="s">
         <v>47</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D29">
+      <c r="D29" s="12">
         <v>1</v>
       </c>
       <c r="E29">
@@ -2203,7 +2228,7 @@
       <c r="K29" s="4"/>
     </row>
     <row r="30" spans="1:11" ht="28.8">
-      <c r="A30" s="9"/>
+      <c r="A30" s="14"/>
       <c r="B30" t="s">
         <v>49</v>
       </c>
@@ -2227,7 +2252,7 @@
       </c>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="9"/>
+      <c r="A31" s="14"/>
       <c r="B31" t="s">
         <v>51</v>
       </c>
@@ -2251,7 +2276,7 @@
       </c>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="9"/>
+      <c r="A32" s="14"/>
       <c r="B32" t="s">
         <v>53</v>
       </c>
@@ -2275,7 +2300,7 @@
       </c>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="9"/>
+      <c r="A33" s="14"/>
       <c r="B33" t="s">
         <v>55</v>
       </c>
@@ -2301,7 +2326,7 @@
       <c r="L33" s="4"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="9"/>
+      <c r="A34" s="14"/>
       <c r="B34" t="s">
         <v>57</v>
       </c>
@@ -2325,7 +2350,7 @@
       </c>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="9"/>
+      <c r="A35" s="14"/>
       <c r="B35" t="s">
         <v>58</v>
       </c>
@@ -2349,14 +2374,14 @@
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="9"/>
+      <c r="A36" s="14"/>
       <c r="B36" t="s">
         <v>60</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D36">
+      <c r="D36" s="12">
         <v>1</v>
       </c>
       <c r="E36">
@@ -2378,7 +2403,7 @@
       <c r="L36" s="4"/>
     </row>
     <row r="37" spans="1:12" ht="28.8">
-      <c r="A37" s="9"/>
+      <c r="A37" s="14"/>
       <c r="B37" t="s">
         <v>61</v>
       </c>
@@ -2402,7 +2427,7 @@
       </c>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="9"/>
+      <c r="A38" s="14"/>
       <c r="B38" t="s">
         <v>63</v>
       </c>
@@ -2426,7 +2451,7 @@
       </c>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="9"/>
+      <c r="A39" s="14"/>
       <c r="B39" t="s">
         <v>65</v>
       </c>
@@ -2450,9 +2475,9 @@
       </c>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="9"/>
-      <c r="B40" s="9"/>
-      <c r="C40" s="9"/>
+      <c r="A40" s="11"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="11"/>
       <c r="D40" s="2" t="s">
         <v>206</v>
       </c>
@@ -2464,13 +2489,13 @@
       </c>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="9" t="s">
+      <c r="A41" s="11" t="s">
         <v>99</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="7" t="s">
         <v>101</v>
       </c>
       <c r="D41">
@@ -2490,11 +2515,11 @@
       </c>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="9"/>
+      <c r="A42" s="11"/>
       <c r="B42" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="7" t="s">
         <v>101</v>
       </c>
       <c r="D42">
@@ -2514,7 +2539,7 @@
       </c>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="9"/>
+      <c r="A43" s="11"/>
       <c r="B43" s="3" t="s">
         <v>105</v>
       </c>
@@ -2538,11 +2563,11 @@
       </c>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="9"/>
+      <c r="A44" s="11"/>
       <c r="B44" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="7" t="s">
         <v>109</v>
       </c>
       <c r="D44">
@@ -2565,11 +2590,11 @@
       </c>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="9"/>
+      <c r="A45" s="11"/>
       <c r="B45" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="7" t="s">
         <v>109</v>
       </c>
       <c r="D45">
@@ -2592,11 +2617,11 @@
       </c>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="9"/>
+      <c r="A46" s="11"/>
       <c r="B46" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="7" t="s">
         <v>114</v>
       </c>
       <c r="D46">
@@ -2616,11 +2641,11 @@
       </c>
     </row>
     <row r="47" spans="1:12">
-      <c r="A47" s="9"/>
+      <c r="A47" s="11"/>
       <c r="B47" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="7" t="s">
         <v>117</v>
       </c>
       <c r="D47">
@@ -2643,11 +2668,11 @@
       </c>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="9"/>
+      <c r="A48" s="11"/>
       <c r="B48" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="7" t="s">
         <v>120</v>
       </c>
       <c r="D48">
@@ -2670,11 +2695,11 @@
       </c>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="9"/>
+      <c r="A49" s="11"/>
       <c r="B49" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="7" t="s">
         <v>122</v>
       </c>
       <c r="D49">
@@ -2694,11 +2719,11 @@
       </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="9"/>
+      <c r="A50" s="11"/>
       <c r="B50" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="7" t="s">
         <v>125</v>
       </c>
       <c r="D50">
@@ -2718,11 +2743,11 @@
       </c>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="9"/>
+      <c r="A51" s="11"/>
       <c r="B51" s="3" t="s">
         <v>126</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="7" t="s">
         <v>127</v>
       </c>
       <c r="D51">
@@ -2745,11 +2770,11 @@
       </c>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="9"/>
+      <c r="A52" s="11"/>
       <c r="B52" t="s">
         <v>129</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="7" t="s">
         <v>127</v>
       </c>
       <c r="D52">
@@ -2772,11 +2797,11 @@
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="9"/>
+      <c r="A53" s="11"/>
       <c r="B53" t="s">
         <v>131</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="7" t="s">
         <v>132</v>
       </c>
       <c r="D53">
@@ -2799,11 +2824,11 @@
       </c>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="9"/>
+      <c r="A54" s="11"/>
       <c r="B54" t="s">
         <v>134</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="7" t="s">
         <v>135</v>
       </c>
       <c r="D54">
@@ -2823,11 +2848,11 @@
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="9"/>
+      <c r="A55" s="11"/>
       <c r="B55" t="s">
         <v>137</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="7" t="s">
         <v>138</v>
       </c>
       <c r="D55">
@@ -2850,11 +2875,11 @@
       </c>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="9"/>
+      <c r="A56" s="11"/>
       <c r="B56" t="s">
         <v>139</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="7" t="s">
         <v>140</v>
       </c>
       <c r="D56">
@@ -2874,11 +2899,11 @@
       </c>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="9"/>
+      <c r="A57" s="11"/>
       <c r="B57" t="s">
         <v>141</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="7" t="s">
         <v>142</v>
       </c>
       <c r="D57">
@@ -2901,11 +2926,11 @@
       </c>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="9"/>
+      <c r="A58" s="11"/>
       <c r="B58" t="s">
         <v>144</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="7" t="s">
         <v>145</v>
       </c>
       <c r="D58">
@@ -2925,11 +2950,11 @@
       </c>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="9"/>
+      <c r="A59" s="11"/>
       <c r="B59" t="s">
         <v>146</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="7" t="s">
         <v>147</v>
       </c>
       <c r="D59">
@@ -2949,11 +2974,11 @@
       </c>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="9"/>
+      <c r="A60" s="11"/>
       <c r="B60" t="s">
         <v>149</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="7" t="s">
         <v>150</v>
       </c>
       <c r="D60">
@@ -2976,11 +3001,11 @@
       </c>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="9"/>
+      <c r="A61" s="11"/>
       <c r="B61" t="s">
         <v>152</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="7" t="s">
         <v>153</v>
       </c>
       <c r="D61">
@@ -3003,11 +3028,11 @@
       </c>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="9"/>
+      <c r="A62" s="11"/>
       <c r="B62" t="s">
         <v>155</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="7" t="s">
         <v>156</v>
       </c>
       <c r="D62">
@@ -3030,11 +3055,11 @@
       </c>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="9"/>
+      <c r="A63" s="11"/>
       <c r="B63" t="s">
         <v>157</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="7" t="s">
         <v>158</v>
       </c>
       <c r="D63">
@@ -3054,11 +3079,11 @@
       </c>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="9"/>
+      <c r="A64" s="11"/>
       <c r="B64" t="s">
         <v>160</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="7" t="s">
         <v>161</v>
       </c>
       <c r="D64">
@@ -3081,11 +3106,11 @@
       </c>
     </row>
     <row r="65" spans="1:9">
-      <c r="A65" s="9"/>
+      <c r="A65" s="11"/>
       <c r="B65" t="s">
         <v>163</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="7" t="s">
         <v>164</v>
       </c>
       <c r="D65">
@@ -3105,11 +3130,11 @@
       </c>
     </row>
     <row r="66" spans="1:9">
-      <c r="A66" s="9"/>
+      <c r="A66" s="11"/>
       <c r="B66" t="s">
         <v>137</v>
       </c>
-      <c r="C66" t="s">
+      <c r="C66" s="7" t="s">
         <v>138</v>
       </c>
       <c r="D66">
@@ -3132,9 +3157,9 @@
       </c>
     </row>
     <row r="67" spans="1:9">
-      <c r="A67" s="9"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
+      <c r="A67" s="11"/>
+      <c r="B67" s="11"/>
+      <c r="C67" s="11"/>
       <c r="D67" s="2" t="s">
         <v>206</v>
       </c>
@@ -3146,13 +3171,13 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="28.8">
-      <c r="A68" s="9" t="s">
+      <c r="A68" s="14" t="s">
         <v>169</v>
       </c>
       <c r="B68" t="s">
         <v>170</v>
       </c>
-      <c r="C68" t="s">
+      <c r="C68" s="10" t="s">
         <v>171</v>
       </c>
       <c r="D68">
@@ -3175,11 +3200,11 @@
       </c>
     </row>
     <row r="69" spans="1:9">
-      <c r="A69" s="9"/>
+      <c r="A69" s="14"/>
       <c r="B69" t="s">
         <v>173</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="8" t="s">
         <v>174</v>
       </c>
       <c r="D69">
@@ -3199,11 +3224,11 @@
       </c>
     </row>
     <row r="70" spans="1:9">
-      <c r="A70" s="9"/>
+      <c r="A70" s="14"/>
       <c r="B70" t="s">
         <v>176</v>
       </c>
-      <c r="C70" t="s">
+      <c r="C70" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D70">
@@ -3226,11 +3251,11 @@
       </c>
     </row>
     <row r="71" spans="1:9">
-      <c r="A71" s="9"/>
+      <c r="A71" s="14"/>
       <c r="B71" t="s">
         <v>178</v>
       </c>
-      <c r="C71" t="s">
+      <c r="C71" s="10" t="s">
         <v>179</v>
       </c>
       <c r="D71">
@@ -3248,16 +3273,16 @@
       <c r="H71">
         <v>3</v>
       </c>
-      <c r="I71" s="6" t="s">
+      <c r="I71" s="9" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="72" spans="1:9" ht="28.8">
-      <c r="A72" s="9"/>
+      <c r="A72" s="14"/>
       <c r="B72" t="s">
         <v>181</v>
       </c>
-      <c r="C72" t="s">
+      <c r="C72" s="10" t="s">
         <v>179</v>
       </c>
       <c r="D72">
@@ -3275,16 +3300,16 @@
       <c r="H72">
         <v>4</v>
       </c>
-      <c r="I72" s="6" t="s">
+      <c r="I72" s="9" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="73" spans="1:9">
-      <c r="A73" s="9"/>
+      <c r="A73" s="14"/>
       <c r="B73" t="s">
         <v>183</v>
       </c>
-      <c r="C73" t="s">
+      <c r="C73" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D73">
@@ -3304,9 +3329,9 @@
       </c>
     </row>
     <row r="74" spans="1:9">
-      <c r="A74" s="9"/>
-      <c r="B74" s="9"/>
-      <c r="C74" s="9"/>
+      <c r="A74" s="11"/>
+      <c r="B74" s="11"/>
+      <c r="C74" s="11"/>
       <c r="D74" s="2" t="s">
         <v>206</v>
       </c>
@@ -3318,13 +3343,13 @@
       </c>
     </row>
     <row r="75" spans="1:9">
-      <c r="A75" s="9" t="s">
+      <c r="A75" s="14" t="s">
         <v>185</v>
       </c>
       <c r="B75" t="s">
         <v>186</v>
       </c>
-      <c r="C75" t="s">
+      <c r="C75" s="10" t="s">
         <v>171</v>
       </c>
       <c r="D75">
@@ -3347,11 +3372,11 @@
       </c>
     </row>
     <row r="76" spans="1:9" ht="28.8">
-      <c r="A76" s="9"/>
+      <c r="A76" s="14"/>
       <c r="B76" t="s">
         <v>188</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D76">
@@ -3374,11 +3399,11 @@
       </c>
     </row>
     <row r="77" spans="1:9">
-      <c r="A77" s="9"/>
+      <c r="A77" s="14"/>
       <c r="B77" t="s">
         <v>189</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="10" t="s">
         <v>17</v>
       </c>
       <c r="D77">
@@ -3401,11 +3426,11 @@
       </c>
     </row>
     <row r="78" spans="1:9">
-      <c r="A78" s="9"/>
+      <c r="A78" s="14"/>
       <c r="B78" t="s">
         <v>176</v>
       </c>
-      <c r="C78" t="s">
+      <c r="C78" s="10" t="s">
         <v>10</v>
       </c>
       <c r="D78">
@@ -3428,11 +3453,11 @@
       </c>
     </row>
     <row r="79" spans="1:9" ht="28.8">
-      <c r="A79" s="9"/>
-      <c r="B79" t="s">
+      <c r="A79" s="14"/>
+      <c r="B79" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="C79" t="s">
+      <c r="C79" s="7" t="s">
         <v>192</v>
       </c>
       <c r="D79">
@@ -3455,11 +3480,11 @@
       </c>
     </row>
     <row r="80" spans="1:9">
-      <c r="A80" s="9"/>
+      <c r="A80" s="14"/>
       <c r="B80" t="s">
         <v>193</v>
       </c>
-      <c r="C80" t="s">
+      <c r="C80" s="7" t="s">
         <v>192</v>
       </c>
       <c r="D80">
@@ -3482,11 +3507,11 @@
       </c>
     </row>
     <row r="81" spans="1:9">
-      <c r="A81" s="9"/>
+      <c r="A81" s="14"/>
       <c r="B81" t="s">
         <v>194</v>
       </c>
-      <c r="C81" t="s">
+      <c r="C81" s="10" t="s">
         <v>195</v>
       </c>
       <c r="D81">
@@ -3509,7 +3534,7 @@
       </c>
     </row>
     <row r="82" spans="1:9">
-      <c r="A82" s="9"/>
+      <c r="A82" s="14"/>
       <c r="B82" t="s">
         <v>197</v>
       </c>
@@ -3536,9 +3561,9 @@
       </c>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="9"/>
-      <c r="B83" s="9"/>
-      <c r="C83" s="9"/>
+      <c r="A83" s="11"/>
+      <c r="B83" s="11"/>
+      <c r="C83" s="11"/>
       <c r="D83" s="2" t="s">
         <v>206</v>
       </c>
@@ -3550,16 +3575,16 @@
       </c>
     </row>
     <row r="84" spans="1:9">
-      <c r="A84" s="9" t="s">
+      <c r="A84" s="14" t="s">
         <v>237</v>
       </c>
       <c r="B84" t="s">
         <v>239</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D84">
+      <c r="D84" s="12">
         <v>0</v>
       </c>
       <c r="E84">
@@ -3579,14 +3604,14 @@
       </c>
     </row>
     <row r="85" spans="1:9">
-      <c r="A85" s="9"/>
+      <c r="A85" s="14"/>
       <c r="B85" t="s">
         <v>238</v>
       </c>
-      <c r="C85" t="s">
+      <c r="C85" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D85">
+      <c r="D85" s="12">
         <v>0</v>
       </c>
       <c r="E85">
@@ -3606,14 +3631,14 @@
       </c>
     </row>
     <row r="86" spans="1:9">
-      <c r="A86" s="9"/>
+      <c r="A86" s="14"/>
       <c r="B86" t="s">
         <v>240</v>
       </c>
-      <c r="C86" t="s">
+      <c r="C86" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="D86">
+      <c r="D86" s="12">
         <v>0</v>
       </c>
       <c r="E86">
@@ -3633,11 +3658,11 @@
       </c>
     </row>
     <row r="87" spans="1:9">
-      <c r="A87" s="9"/>
+      <c r="A87" s="14"/>
       <c r="B87" t="s">
         <v>242</v>
       </c>
-      <c r="C87" t="s">
+      <c r="C87" s="7" t="s">
         <v>250</v>
       </c>
       <c r="D87">
@@ -3660,11 +3685,11 @@
       </c>
     </row>
     <row r="88" spans="1:9">
-      <c r="A88" s="9"/>
+      <c r="A88" s="14"/>
       <c r="B88" t="s">
         <v>243</v>
       </c>
-      <c r="C88" t="s">
+      <c r="C88" s="7" t="s">
         <v>251</v>
       </c>
       <c r="D88">
@@ -3687,11 +3712,11 @@
       </c>
     </row>
     <row r="89" spans="1:9">
-      <c r="A89" s="9"/>
+      <c r="A89" s="14"/>
       <c r="B89" t="s">
         <v>244</v>
       </c>
-      <c r="C89" t="s">
+      <c r="C89" s="7" t="s">
         <v>252</v>
       </c>
       <c r="D89">
@@ -3714,11 +3739,11 @@
       </c>
     </row>
     <row r="90" spans="1:9">
-      <c r="A90" s="9"/>
+      <c r="A90" s="14"/>
       <c r="B90" t="s">
         <v>245</v>
       </c>
-      <c r="C90" t="s">
+      <c r="C90" s="7" t="s">
         <v>249</v>
       </c>
       <c r="D90">
@@ -3738,11 +3763,11 @@
       </c>
     </row>
     <row r="91" spans="1:9">
-      <c r="A91" s="9"/>
+      <c r="A91" s="14"/>
       <c r="B91" t="s">
         <v>60</v>
       </c>
-      <c r="C91" t="s">
+      <c r="C91" s="10" t="s">
         <v>48</v>
       </c>
       <c r="D91">
@@ -3765,7 +3790,7 @@
       </c>
     </row>
     <row r="92" spans="1:9">
-      <c r="A92" s="9"/>
+      <c r="A92" s="14"/>
       <c r="B92" t="s">
         <v>246</v>
       </c>
@@ -3789,7 +3814,7 @@
       </c>
     </row>
     <row r="93" spans="1:9">
-      <c r="A93" s="9"/>
+      <c r="A93" s="14"/>
       <c r="B93" t="s">
         <v>247</v>
       </c>
@@ -3813,7 +3838,7 @@
       </c>
     </row>
     <row r="94" spans="1:9">
-      <c r="A94" s="9"/>
+      <c r="A94" s="14"/>
       <c r="D94" s="2" t="s">
         <v>206</v>
       </c>
@@ -3825,7 +3850,7 @@
       </c>
     </row>
     <row r="97" spans="1:9" ht="43.2">
-      <c r="A97" s="9" t="s">
+      <c r="A97" s="11" t="s">
         <v>264</v>
       </c>
       <c r="B97" t="s">
@@ -3851,7 +3876,7 @@
       </c>
     </row>
     <row r="98" spans="1:9">
-      <c r="A98" s="9"/>
+      <c r="A98" s="11"/>
       <c r="B98" t="s">
         <v>266</v>
       </c>
@@ -3875,7 +3900,7 @@
       </c>
     </row>
     <row r="99" spans="1:9">
-      <c r="A99" s="9"/>
+      <c r="A99" s="11"/>
       <c r="B99" t="s">
         <v>267</v>
       </c>
@@ -3899,7 +3924,7 @@
       </c>
     </row>
     <row r="100" spans="1:9">
-      <c r="A100" s="9"/>
+      <c r="A100" s="11"/>
       <c r="B100" t="s">
         <v>268</v>
       </c>
@@ -3923,7 +3948,7 @@
       </c>
     </row>
     <row r="101" spans="1:9">
-      <c r="A101" s="9"/>
+      <c r="A101" s="11"/>
       <c r="B101" t="s">
         <v>269</v>
       </c>
@@ -3947,7 +3972,7 @@
       </c>
     </row>
     <row r="102" spans="1:9">
-      <c r="A102" s="9"/>
+      <c r="A102" s="11"/>
       <c r="B102" t="s">
         <v>270</v>
       </c>
@@ -3971,7 +3996,7 @@
       </c>
     </row>
     <row r="103" spans="1:9">
-      <c r="A103" s="9"/>
+      <c r="A103" s="11"/>
       <c r="B103" t="s">
         <v>271</v>
       </c>
@@ -3995,7 +4020,7 @@
       </c>
     </row>
     <row r="104" spans="1:9">
-      <c r="A104" s="9"/>
+      <c r="A104" s="11"/>
       <c r="B104" t="s">
         <v>272</v>
       </c>
@@ -4019,7 +4044,7 @@
       </c>
     </row>
     <row r="105" spans="1:9">
-      <c r="A105" s="9"/>
+      <c r="A105" s="11"/>
       <c r="B105" t="s">
         <v>263</v>
       </c>
@@ -4043,7 +4068,7 @@
       </c>
     </row>
     <row r="106" spans="1:9">
-      <c r="A106" s="9"/>
+      <c r="A106" s="11"/>
       <c r="B106" t="s">
         <v>273</v>
       </c>
@@ -4067,7 +4092,7 @@
       </c>
     </row>
     <row r="107" spans="1:9">
-      <c r="A107" s="9"/>
+      <c r="A107" s="11"/>
       <c r="B107" t="s">
         <v>274</v>
       </c>
@@ -4091,7 +4116,7 @@
       </c>
     </row>
     <row r="108" spans="1:9">
-      <c r="A108" s="9"/>
+      <c r="A108" s="11"/>
       <c r="B108" t="s">
         <v>275</v>
       </c>
@@ -4115,7 +4140,7 @@
       </c>
     </row>
     <row r="109" spans="1:9">
-      <c r="A109" s="9"/>
+      <c r="A109" s="11"/>
       <c r="B109" t="s">
         <v>276</v>
       </c>
@@ -4139,7 +4164,7 @@
       </c>
     </row>
     <row r="110" spans="1:9">
-      <c r="A110" s="9"/>
+      <c r="A110" s="11"/>
       <c r="B110" t="s">
         <v>277</v>
       </c>
@@ -4163,7 +4188,7 @@
       </c>
     </row>
     <row r="111" spans="1:9">
-      <c r="A111" s="9"/>
+      <c r="A111" s="11"/>
       <c r="B111" t="s">
         <v>278</v>
       </c>
@@ -4187,7 +4212,7 @@
       </c>
     </row>
     <row r="112" spans="1:9">
-      <c r="A112" s="9"/>
+      <c r="A112" s="11"/>
       <c r="B112" t="s">
         <v>279</v>
       </c>
@@ -4211,7 +4236,7 @@
       </c>
     </row>
     <row r="113" spans="1:9">
-      <c r="A113" s="9"/>
+      <c r="A113" s="11"/>
       <c r="B113" t="s">
         <v>160</v>
       </c>
@@ -4235,7 +4260,7 @@
       </c>
     </row>
     <row r="114" spans="1:9">
-      <c r="A114" s="9"/>
+      <c r="A114" s="11"/>
       <c r="B114" t="s">
         <v>280</v>
       </c>
@@ -4259,7 +4284,7 @@
       </c>
     </row>
     <row r="115" spans="1:9">
-      <c r="A115" s="9"/>
+      <c r="A115" s="11"/>
       <c r="B115" t="s">
         <v>281</v>
       </c>
@@ -4283,7 +4308,7 @@
       </c>
     </row>
     <row r="116" spans="1:9">
-      <c r="A116" s="9"/>
+      <c r="A116" s="11"/>
       <c r="B116" t="s">
         <v>282</v>
       </c>
@@ -4307,7 +4332,7 @@
       </c>
     </row>
     <row r="117" spans="1:9">
-      <c r="A117" s="9"/>
+      <c r="A117" s="11"/>
       <c r="B117" t="s">
         <v>283</v>
       </c>
@@ -4331,7 +4356,7 @@
       </c>
     </row>
     <row r="118" spans="1:9">
-      <c r="A118" s="9"/>
+      <c r="A118" s="11"/>
       <c r="B118" t="s">
         <v>284</v>
       </c>
@@ -4355,7 +4380,7 @@
       </c>
     </row>
     <row r="119" spans="1:9">
-      <c r="A119" s="9"/>
+      <c r="A119" s="11"/>
       <c r="B119" t="s">
         <v>285</v>
       </c>
@@ -4379,7 +4404,7 @@
       </c>
     </row>
     <row r="120" spans="1:9">
-      <c r="A120" s="9"/>
+      <c r="A120" s="11"/>
       <c r="B120" t="s">
         <v>286</v>
       </c>
@@ -4403,7 +4428,7 @@
       </c>
     </row>
     <row r="121" spans="1:9">
-      <c r="A121" s="9"/>
+      <c r="A121" s="11"/>
       <c r="D121" t="s">
         <v>206</v>
       </c>

</xml_diff>

<commit_message>
MUSE excell sheet modified
</commit_message>
<xml_diff>
--- a/CodeKernel_Manual_Data/MUSE Data/labels_muse.xlsx
+++ b/CodeKernel_Manual_Data/MUSE Data/labels_muse.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26327"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26FA17E4-7C34-4A9D-9160-8F1505E57786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6225643-D182-4A40-9C40-B6C102B2F04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="328">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="439" uniqueCount="331">
   <si>
     <t>API</t>
   </si>
@@ -1003,6 +1003,15 @@
   <si>
     <t>basesim</t>
     <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>My Note</t>
+  </si>
+  <si>
+    <t>Have modified 4 such that they will have only one API call each.</t>
+  </si>
+  <si>
+    <t>Have modified 5 such that they will have only one API call each.</t>
   </si>
 </sst>
 </file>
@@ -1101,7 +1110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1121,12 +1130,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1470,8 +1478,8 @@
   <dimension ref="A1:L121"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A75" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A75" sqref="A75:A82"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -1481,10 +1489,10 @@
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
     <col min="7" max="8" width="9.109375" customWidth="1"/>
     <col min="9" max="9" width="56.109375" style="6" customWidth="1"/>
-    <col min="10" max="10" width="8.77734375" customWidth="1"/>
+    <col min="10" max="10" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1">
+    <row r="1" spans="1:10" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1512,9 +1520,12 @@
       <c r="I1" s="5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" s="14" t="s">
+      <c r="J1" s="1" t="s">
+        <v>328</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="B2" t="s">
@@ -1542,8 +1553,8 @@
         <v>87</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="14"/>
+    <row r="3" spans="1:10">
+      <c r="A3" s="12"/>
       <c r="B3" t="s">
         <v>7</v>
       </c>
@@ -1569,15 +1580,15 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="28.8">
-      <c r="A4" s="14"/>
-      <c r="B4" s="13" t="s">
+    <row r="4" spans="1:10" ht="28.8">
+      <c r="A4" s="12"/>
+      <c r="B4" s="11" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="12">
+      <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
@@ -1595,16 +1606,19 @@
       <c r="I4" s="6" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="28.8">
-      <c r="A5" s="14"/>
-      <c r="B5" s="13" t="s">
+      <c r="J4" s="6" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="28.8">
+      <c r="A5" s="12"/>
+      <c r="B5" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="12">
+      <c r="D5">
         <v>1</v>
       </c>
       <c r="E5">
@@ -1619,9 +1633,12 @@
       <c r="I5" s="6" t="s">
         <v>90</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="43.2">
-      <c r="A6" s="14"/>
+      <c r="J5" s="6" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="43.2">
+      <c r="A6" s="12"/>
       <c r="B6" t="s">
         <v>12</v>
       </c>
@@ -1647,8 +1664,8 @@
         <v>91</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="14"/>
+    <row r="7" spans="1:10">
+      <c r="A7" s="12"/>
       <c r="B7" t="s">
         <v>14</v>
       </c>
@@ -1674,15 +1691,15 @@
         <v>92</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="14"/>
+    <row r="8" spans="1:10">
+      <c r="A8" s="12"/>
       <c r="B8" t="s">
         <v>19</v>
       </c>
       <c r="C8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="12">
+      <c r="D8">
         <v>1</v>
       </c>
       <c r="E8">
@@ -1698,15 +1715,15 @@
         <v>94</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="14"/>
+    <row r="9" spans="1:10">
+      <c r="A9" s="12"/>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="12">
+      <c r="D9">
         <v>3</v>
       </c>
       <c r="E9">
@@ -1725,8 +1742,8 @@
         <v>96</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
-      <c r="A10" s="14"/>
+    <row r="10" spans="1:10">
+      <c r="A10" s="12"/>
       <c r="B10" t="s">
         <v>21</v>
       </c>
@@ -1749,8 +1766,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
-      <c r="A11" s="14"/>
+    <row r="11" spans="1:10">
+      <c r="A11" s="12"/>
       <c r="B11" t="s">
         <v>22</v>
       </c>
@@ -1773,8 +1790,8 @@
         <v>93</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
-      <c r="A12" s="14"/>
+    <row r="12" spans="1:10">
+      <c r="A12" s="12"/>
       <c r="B12" t="s">
         <v>23</v>
       </c>
@@ -1797,15 +1814,15 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="14"/>
+    <row r="13" spans="1:10">
+      <c r="A13" s="12"/>
       <c r="B13" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="12">
+      <c r="D13">
         <v>2</v>
       </c>
       <c r="E13">
@@ -1821,10 +1838,10 @@
         <v>95</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="11"/>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
+    <row r="14" spans="1:10">
+      <c r="A14" s="13"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="2" t="s">
         <v>206</v>
       </c>
@@ -1835,8 +1852,8 @@
         <v>211</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="14" t="s">
+    <row r="15" spans="1:10">
+      <c r="A15" s="12" t="s">
         <v>28</v>
       </c>
       <c r="B15" t="s">
@@ -1864,15 +1881,15 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="14"/>
-      <c r="B16" s="13" t="s">
+    <row r="16" spans="1:10">
+      <c r="A16" s="12"/>
+      <c r="B16" s="11" t="s">
         <v>166</v>
       </c>
       <c r="C16" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="12">
+      <c r="D16">
         <v>0</v>
       </c>
       <c r="E16">
@@ -1889,7 +1906,7 @@
       </c>
     </row>
     <row r="17" spans="1:11">
-      <c r="A17" s="14"/>
+      <c r="A17" s="12"/>
       <c r="B17" t="s">
         <v>31</v>
       </c>
@@ -1916,7 +1933,7 @@
       </c>
     </row>
     <row r="18" spans="1:11">
-      <c r="A18" s="14"/>
+      <c r="A18" s="12"/>
       <c r="B18" t="s">
         <v>33</v>
       </c>
@@ -1943,7 +1960,7 @@
       </c>
     </row>
     <row r="19" spans="1:11">
-      <c r="A19" s="14"/>
+      <c r="A19" s="12"/>
       <c r="B19" t="s">
         <v>35</v>
       </c>
@@ -1967,14 +1984,14 @@
       </c>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="14"/>
+      <c r="A20" s="12"/>
       <c r="B20" t="s">
         <v>36</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>37</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20">
         <v>1</v>
       </c>
       <c r="E20">
@@ -1994,14 +2011,14 @@
       </c>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="14"/>
+      <c r="A21" s="12"/>
       <c r="B21" t="s">
         <v>38</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="D21" s="12">
+      <c r="D21">
         <v>4</v>
       </c>
       <c r="E21">
@@ -2021,7 +2038,7 @@
       </c>
     </row>
     <row r="22" spans="1:11">
-      <c r="A22" s="14"/>
+      <c r="A22" s="12"/>
       <c r="B22" t="s">
         <v>40</v>
       </c>
@@ -2047,7 +2064,7 @@
       <c r="K22" s="4"/>
     </row>
     <row r="23" spans="1:11">
-      <c r="A23" s="14"/>
+      <c r="A23" s="12"/>
       <c r="B23" t="s">
         <v>42</v>
       </c>
@@ -2074,7 +2091,7 @@
       </c>
     </row>
     <row r="24" spans="1:11">
-      <c r="A24" s="14"/>
+      <c r="A24" s="12"/>
       <c r="B24" t="s">
         <v>44</v>
       </c>
@@ -2098,14 +2115,14 @@
       </c>
     </row>
     <row r="25" spans="1:11">
-      <c r="A25" s="14"/>
+      <c r="A25" s="12"/>
       <c r="B25" t="s">
         <v>45</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="12">
+      <c r="D25">
         <v>1</v>
       </c>
       <c r="E25">
@@ -2122,14 +2139,14 @@
       </c>
     </row>
     <row r="26" spans="1:11">
-      <c r="A26" s="14"/>
-      <c r="B26" s="13" t="s">
+      <c r="A26" s="12"/>
+      <c r="B26" s="11" t="s">
         <v>167</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="12">
+      <c r="D26">
         <v>1</v>
       </c>
       <c r="E26">
@@ -2146,14 +2163,14 @@
       </c>
     </row>
     <row r="27" spans="1:11">
-      <c r="A27" s="14"/>
+      <c r="A27" s="12"/>
       <c r="B27" t="s">
         <v>168</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D27" s="12">
+      <c r="D27">
         <v>0</v>
       </c>
       <c r="E27">
@@ -2170,14 +2187,14 @@
       </c>
     </row>
     <row r="28" spans="1:11">
-      <c r="A28" s="14"/>
+      <c r="A28" s="12"/>
       <c r="B28" t="s">
         <v>46</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="D28" s="12">
+      <c r="D28">
         <v>1</v>
       </c>
       <c r="E28">
@@ -2199,14 +2216,14 @@
       <c r="K28" s="4"/>
     </row>
     <row r="29" spans="1:11">
-      <c r="A29" s="14"/>
+      <c r="A29" s="12"/>
       <c r="B29" t="s">
         <v>47</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D29" s="12">
+      <c r="D29">
         <v>1</v>
       </c>
       <c r="E29">
@@ -2228,7 +2245,7 @@
       <c r="K29" s="4"/>
     </row>
     <row r="30" spans="1:11" ht="28.8">
-      <c r="A30" s="14"/>
+      <c r="A30" s="12"/>
       <c r="B30" t="s">
         <v>49</v>
       </c>
@@ -2252,7 +2269,7 @@
       </c>
     </row>
     <row r="31" spans="1:11">
-      <c r="A31" s="14"/>
+      <c r="A31" s="12"/>
       <c r="B31" t="s">
         <v>51</v>
       </c>
@@ -2276,7 +2293,7 @@
       </c>
     </row>
     <row r="32" spans="1:11">
-      <c r="A32" s="14"/>
+      <c r="A32" s="12"/>
       <c r="B32" t="s">
         <v>53</v>
       </c>
@@ -2300,7 +2317,7 @@
       </c>
     </row>
     <row r="33" spans="1:12">
-      <c r="A33" s="14"/>
+      <c r="A33" s="12"/>
       <c r="B33" t="s">
         <v>55</v>
       </c>
@@ -2326,7 +2343,7 @@
       <c r="L33" s="4"/>
     </row>
     <row r="34" spans="1:12">
-      <c r="A34" s="14"/>
+      <c r="A34" s="12"/>
       <c r="B34" t="s">
         <v>57</v>
       </c>
@@ -2350,7 +2367,7 @@
       </c>
     </row>
     <row r="35" spans="1:12">
-      <c r="A35" s="14"/>
+      <c r="A35" s="12"/>
       <c r="B35" t="s">
         <v>58</v>
       </c>
@@ -2374,14 +2391,14 @@
       </c>
     </row>
     <row r="36" spans="1:12">
-      <c r="A36" s="14"/>
+      <c r="A36" s="12"/>
       <c r="B36" t="s">
         <v>60</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="D36" s="12">
+      <c r="D36">
         <v>1</v>
       </c>
       <c r="E36">
@@ -2403,7 +2420,7 @@
       <c r="L36" s="4"/>
     </row>
     <row r="37" spans="1:12" ht="28.8">
-      <c r="A37" s="14"/>
+      <c r="A37" s="12"/>
       <c r="B37" t="s">
         <v>61</v>
       </c>
@@ -2427,7 +2444,7 @@
       </c>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="14"/>
+      <c r="A38" s="12"/>
       <c r="B38" t="s">
         <v>63</v>
       </c>
@@ -2451,7 +2468,7 @@
       </c>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="14"/>
+      <c r="A39" s="12"/>
       <c r="B39" t="s">
         <v>65</v>
       </c>
@@ -2475,9 +2492,9 @@
       </c>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="11"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="11"/>
+      <c r="A40" s="13"/>
+      <c r="B40" s="13"/>
+      <c r="C40" s="13"/>
       <c r="D40" s="2" t="s">
         <v>206</v>
       </c>
@@ -2489,7 +2506,7 @@
       </c>
     </row>
     <row r="41" spans="1:12">
-      <c r="A41" s="11" t="s">
+      <c r="A41" s="13" t="s">
         <v>99</v>
       </c>
       <c r="B41" s="3" t="s">
@@ -2515,7 +2532,7 @@
       </c>
     </row>
     <row r="42" spans="1:12">
-      <c r="A42" s="11"/>
+      <c r="A42" s="13"/>
       <c r="B42" s="3" t="s">
         <v>103</v>
       </c>
@@ -2539,7 +2556,7 @@
       </c>
     </row>
     <row r="43" spans="1:12">
-      <c r="A43" s="11"/>
+      <c r="A43" s="13"/>
       <c r="B43" s="3" t="s">
         <v>105</v>
       </c>
@@ -2563,7 +2580,7 @@
       </c>
     </row>
     <row r="44" spans="1:12">
-      <c r="A44" s="11"/>
+      <c r="A44" s="13"/>
       <c r="B44" s="3" t="s">
         <v>108</v>
       </c>
@@ -2590,7 +2607,7 @@
       </c>
     </row>
     <row r="45" spans="1:12">
-      <c r="A45" s="11"/>
+      <c r="A45" s="13"/>
       <c r="B45" s="3" t="s">
         <v>111</v>
       </c>
@@ -2617,7 +2634,7 @@
       </c>
     </row>
     <row r="46" spans="1:12">
-      <c r="A46" s="11"/>
+      <c r="A46" s="13"/>
       <c r="B46" s="3" t="s">
         <v>113</v>
       </c>
@@ -2641,7 +2658,7 @@
       </c>
     </row>
     <row r="47" spans="1:12">
-      <c r="A47" s="11"/>
+      <c r="A47" s="13"/>
       <c r="B47" s="3" t="s">
         <v>116</v>
       </c>
@@ -2668,7 +2685,7 @@
       </c>
     </row>
     <row r="48" spans="1:12">
-      <c r="A48" s="11"/>
+      <c r="A48" s="13"/>
       <c r="B48" s="3" t="s">
         <v>119</v>
       </c>
@@ -2695,7 +2712,7 @@
       </c>
     </row>
     <row r="49" spans="1:9">
-      <c r="A49" s="11"/>
+      <c r="A49" s="13"/>
       <c r="B49" s="3" t="s">
         <v>121</v>
       </c>
@@ -2719,7 +2736,7 @@
       </c>
     </row>
     <row r="50" spans="1:9">
-      <c r="A50" s="11"/>
+      <c r="A50" s="13"/>
       <c r="B50" s="3" t="s">
         <v>124</v>
       </c>
@@ -2743,7 +2760,7 @@
       </c>
     </row>
     <row r="51" spans="1:9">
-      <c r="A51" s="11"/>
+      <c r="A51" s="13"/>
       <c r="B51" s="3" t="s">
         <v>126</v>
       </c>
@@ -2770,7 +2787,7 @@
       </c>
     </row>
     <row r="52" spans="1:9">
-      <c r="A52" s="11"/>
+      <c r="A52" s="13"/>
       <c r="B52" t="s">
         <v>129</v>
       </c>
@@ -2797,7 +2814,7 @@
       </c>
     </row>
     <row r="53" spans="1:9">
-      <c r="A53" s="11"/>
+      <c r="A53" s="13"/>
       <c r="B53" t="s">
         <v>131</v>
       </c>
@@ -2824,7 +2841,7 @@
       </c>
     </row>
     <row r="54" spans="1:9">
-      <c r="A54" s="11"/>
+      <c r="A54" s="13"/>
       <c r="B54" t="s">
         <v>134</v>
       </c>
@@ -2848,7 +2865,7 @@
       </c>
     </row>
     <row r="55" spans="1:9">
-      <c r="A55" s="11"/>
+      <c r="A55" s="13"/>
       <c r="B55" t="s">
         <v>137</v>
       </c>
@@ -2875,7 +2892,7 @@
       </c>
     </row>
     <row r="56" spans="1:9">
-      <c r="A56" s="11"/>
+      <c r="A56" s="13"/>
       <c r="B56" t="s">
         <v>139</v>
       </c>
@@ -2899,7 +2916,7 @@
       </c>
     </row>
     <row r="57" spans="1:9">
-      <c r="A57" s="11"/>
+      <c r="A57" s="13"/>
       <c r="B57" t="s">
         <v>141</v>
       </c>
@@ -2926,7 +2943,7 @@
       </c>
     </row>
     <row r="58" spans="1:9">
-      <c r="A58" s="11"/>
+      <c r="A58" s="13"/>
       <c r="B58" t="s">
         <v>144</v>
       </c>
@@ -2950,7 +2967,7 @@
       </c>
     </row>
     <row r="59" spans="1:9">
-      <c r="A59" s="11"/>
+      <c r="A59" s="13"/>
       <c r="B59" t="s">
         <v>146</v>
       </c>
@@ -2974,7 +2991,7 @@
       </c>
     </row>
     <row r="60" spans="1:9">
-      <c r="A60" s="11"/>
+      <c r="A60" s="13"/>
       <c r="B60" t="s">
         <v>149</v>
       </c>
@@ -3001,7 +3018,7 @@
       </c>
     </row>
     <row r="61" spans="1:9">
-      <c r="A61" s="11"/>
+      <c r="A61" s="13"/>
       <c r="B61" t="s">
         <v>152</v>
       </c>
@@ -3028,7 +3045,7 @@
       </c>
     </row>
     <row r="62" spans="1:9">
-      <c r="A62" s="11"/>
+      <c r="A62" s="13"/>
       <c r="B62" t="s">
         <v>155</v>
       </c>
@@ -3055,7 +3072,7 @@
       </c>
     </row>
     <row r="63" spans="1:9">
-      <c r="A63" s="11"/>
+      <c r="A63" s="13"/>
       <c r="B63" t="s">
         <v>157</v>
       </c>
@@ -3079,7 +3096,7 @@
       </c>
     </row>
     <row r="64" spans="1:9">
-      <c r="A64" s="11"/>
+      <c r="A64" s="13"/>
       <c r="B64" t="s">
         <v>160</v>
       </c>
@@ -3106,7 +3123,7 @@
       </c>
     </row>
     <row r="65" spans="1:9">
-      <c r="A65" s="11"/>
+      <c r="A65" s="13"/>
       <c r="B65" t="s">
         <v>163</v>
       </c>
@@ -3130,7 +3147,7 @@
       </c>
     </row>
     <row r="66" spans="1:9">
-      <c r="A66" s="11"/>
+      <c r="A66" s="13"/>
       <c r="B66" t="s">
         <v>137</v>
       </c>
@@ -3157,9 +3174,9 @@
       </c>
     </row>
     <row r="67" spans="1:9">
-      <c r="A67" s="11"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="11"/>
+      <c r="A67" s="13"/>
+      <c r="B67" s="13"/>
+      <c r="C67" s="13"/>
       <c r="D67" s="2" t="s">
         <v>206</v>
       </c>
@@ -3171,7 +3188,7 @@
       </c>
     </row>
     <row r="68" spans="1:9" ht="28.8">
-      <c r="A68" s="14" t="s">
+      <c r="A68" s="12" t="s">
         <v>169</v>
       </c>
       <c r="B68" t="s">
@@ -3200,7 +3217,7 @@
       </c>
     </row>
     <row r="69" spans="1:9">
-      <c r="A69" s="14"/>
+      <c r="A69" s="12"/>
       <c r="B69" t="s">
         <v>173</v>
       </c>
@@ -3224,7 +3241,7 @@
       </c>
     </row>
     <row r="70" spans="1:9">
-      <c r="A70" s="14"/>
+      <c r="A70" s="12"/>
       <c r="B70" t="s">
         <v>176</v>
       </c>
@@ -3251,7 +3268,7 @@
       </c>
     </row>
     <row r="71" spans="1:9">
-      <c r="A71" s="14"/>
+      <c r="A71" s="12"/>
       <c r="B71" t="s">
         <v>178</v>
       </c>
@@ -3278,7 +3295,7 @@
       </c>
     </row>
     <row r="72" spans="1:9" ht="28.8">
-      <c r="A72" s="14"/>
+      <c r="A72" s="12"/>
       <c r="B72" t="s">
         <v>181</v>
       </c>
@@ -3305,7 +3322,7 @@
       </c>
     </row>
     <row r="73" spans="1:9">
-      <c r="A73" s="14"/>
+      <c r="A73" s="12"/>
       <c r="B73" t="s">
         <v>183</v>
       </c>
@@ -3329,9 +3346,9 @@
       </c>
     </row>
     <row r="74" spans="1:9">
-      <c r="A74" s="11"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="11"/>
+      <c r="A74" s="13"/>
+      <c r="B74" s="13"/>
+      <c r="C74" s="13"/>
       <c r="D74" s="2" t="s">
         <v>206</v>
       </c>
@@ -3343,7 +3360,7 @@
       </c>
     </row>
     <row r="75" spans="1:9">
-      <c r="A75" s="14" t="s">
+      <c r="A75" s="12" t="s">
         <v>185</v>
       </c>
       <c r="B75" t="s">
@@ -3372,7 +3389,7 @@
       </c>
     </row>
     <row r="76" spans="1:9" ht="28.8">
-      <c r="A76" s="14"/>
+      <c r="A76" s="12"/>
       <c r="B76" t="s">
         <v>188</v>
       </c>
@@ -3399,7 +3416,7 @@
       </c>
     </row>
     <row r="77" spans="1:9">
-      <c r="A77" s="14"/>
+      <c r="A77" s="12"/>
       <c r="B77" t="s">
         <v>189</v>
       </c>
@@ -3426,7 +3443,7 @@
       </c>
     </row>
     <row r="78" spans="1:9">
-      <c r="A78" s="14"/>
+      <c r="A78" s="12"/>
       <c r="B78" t="s">
         <v>176</v>
       </c>
@@ -3453,8 +3470,8 @@
       </c>
     </row>
     <row r="79" spans="1:9" ht="28.8">
-      <c r="A79" s="14"/>
-      <c r="B79" s="12" t="s">
+      <c r="A79" s="12"/>
+      <c r="B79" t="s">
         <v>191</v>
       </c>
       <c r="C79" s="7" t="s">
@@ -3480,7 +3497,7 @@
       </c>
     </row>
     <row r="80" spans="1:9">
-      <c r="A80" s="14"/>
+      <c r="A80" s="12"/>
       <c r="B80" t="s">
         <v>193</v>
       </c>
@@ -3507,7 +3524,7 @@
       </c>
     </row>
     <row r="81" spans="1:9">
-      <c r="A81" s="14"/>
+      <c r="A81" s="12"/>
       <c r="B81" t="s">
         <v>194</v>
       </c>
@@ -3534,7 +3551,7 @@
       </c>
     </row>
     <row r="82" spans="1:9">
-      <c r="A82" s="14"/>
+      <c r="A82" s="12"/>
       <c r="B82" t="s">
         <v>197</v>
       </c>
@@ -3561,9 +3578,9 @@
       </c>
     </row>
     <row r="83" spans="1:9">
-      <c r="A83" s="11"/>
-      <c r="B83" s="11"/>
-      <c r="C83" s="11"/>
+      <c r="A83" s="13"/>
+      <c r="B83" s="13"/>
+      <c r="C83" s="13"/>
       <c r="D83" s="2" t="s">
         <v>206</v>
       </c>
@@ -3575,7 +3592,7 @@
       </c>
     </row>
     <row r="84" spans="1:9">
-      <c r="A84" s="14" t="s">
+      <c r="A84" s="12" t="s">
         <v>237</v>
       </c>
       <c r="B84" t="s">
@@ -3584,7 +3601,7 @@
       <c r="C84" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D84" s="12">
+      <c r="D84">
         <v>0</v>
       </c>
       <c r="E84">
@@ -3604,14 +3621,14 @@
       </c>
     </row>
     <row r="85" spans="1:9">
-      <c r="A85" s="14"/>
+      <c r="A85" s="12"/>
       <c r="B85" t="s">
         <v>238</v>
       </c>
       <c r="C85" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D85" s="12">
+      <c r="D85">
         <v>0</v>
       </c>
       <c r="E85">
@@ -3631,14 +3648,14 @@
       </c>
     </row>
     <row r="86" spans="1:9">
-      <c r="A86" s="14"/>
+      <c r="A86" s="12"/>
       <c r="B86" t="s">
         <v>240</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>241</v>
       </c>
-      <c r="D86" s="12">
+      <c r="D86">
         <v>0</v>
       </c>
       <c r="E86">
@@ -3658,7 +3675,7 @@
       </c>
     </row>
     <row r="87" spans="1:9">
-      <c r="A87" s="14"/>
+      <c r="A87" s="12"/>
       <c r="B87" t="s">
         <v>242</v>
       </c>
@@ -3685,7 +3702,7 @@
       </c>
     </row>
     <row r="88" spans="1:9">
-      <c r="A88" s="14"/>
+      <c r="A88" s="12"/>
       <c r="B88" t="s">
         <v>243</v>
       </c>
@@ -3712,7 +3729,7 @@
       </c>
     </row>
     <row r="89" spans="1:9">
-      <c r="A89" s="14"/>
+      <c r="A89" s="12"/>
       <c r="B89" t="s">
         <v>244</v>
       </c>
@@ -3739,7 +3756,7 @@
       </c>
     </row>
     <row r="90" spans="1:9">
-      <c r="A90" s="14"/>
+      <c r="A90" s="12"/>
       <c r="B90" t="s">
         <v>245</v>
       </c>
@@ -3763,7 +3780,7 @@
       </c>
     </row>
     <row r="91" spans="1:9">
-      <c r="A91" s="14"/>
+      <c r="A91" s="12"/>
       <c r="B91" t="s">
         <v>60</v>
       </c>
@@ -3790,7 +3807,7 @@
       </c>
     </row>
     <row r="92" spans="1:9">
-      <c r="A92" s="14"/>
+      <c r="A92" s="12"/>
       <c r="B92" t="s">
         <v>246</v>
       </c>
@@ -3814,7 +3831,7 @@
       </c>
     </row>
     <row r="93" spans="1:9">
-      <c r="A93" s="14"/>
+      <c r="A93" s="12"/>
       <c r="B93" t="s">
         <v>247</v>
       </c>
@@ -3838,7 +3855,7 @@
       </c>
     </row>
     <row r="94" spans="1:9">
-      <c r="A94" s="14"/>
+      <c r="A94" s="12"/>
       <c r="D94" s="2" t="s">
         <v>206</v>
       </c>
@@ -3850,7 +3867,7 @@
       </c>
     </row>
     <row r="97" spans="1:9" ht="43.2">
-      <c r="A97" s="11" t="s">
+      <c r="A97" s="13" t="s">
         <v>264</v>
       </c>
       <c r="B97" t="s">
@@ -3876,7 +3893,7 @@
       </c>
     </row>
     <row r="98" spans="1:9">
-      <c r="A98" s="11"/>
+      <c r="A98" s="13"/>
       <c r="B98" t="s">
         <v>266</v>
       </c>
@@ -3900,7 +3917,7 @@
       </c>
     </row>
     <row r="99" spans="1:9">
-      <c r="A99" s="11"/>
+      <c r="A99" s="13"/>
       <c r="B99" t="s">
         <v>267</v>
       </c>
@@ -3924,7 +3941,7 @@
       </c>
     </row>
     <row r="100" spans="1:9">
-      <c r="A100" s="11"/>
+      <c r="A100" s="13"/>
       <c r="B100" t="s">
         <v>268</v>
       </c>
@@ -3948,7 +3965,7 @@
       </c>
     </row>
     <row r="101" spans="1:9">
-      <c r="A101" s="11"/>
+      <c r="A101" s="13"/>
       <c r="B101" t="s">
         <v>269</v>
       </c>
@@ -3972,7 +3989,7 @@
       </c>
     </row>
     <row r="102" spans="1:9">
-      <c r="A102" s="11"/>
+      <c r="A102" s="13"/>
       <c r="B102" t="s">
         <v>270</v>
       </c>
@@ -3996,7 +4013,7 @@
       </c>
     </row>
     <row r="103" spans="1:9">
-      <c r="A103" s="11"/>
+      <c r="A103" s="13"/>
       <c r="B103" t="s">
         <v>271</v>
       </c>
@@ -4020,7 +4037,7 @@
       </c>
     </row>
     <row r="104" spans="1:9">
-      <c r="A104" s="11"/>
+      <c r="A104" s="13"/>
       <c r="B104" t="s">
         <v>272</v>
       </c>
@@ -4044,7 +4061,7 @@
       </c>
     </row>
     <row r="105" spans="1:9">
-      <c r="A105" s="11"/>
+      <c r="A105" s="13"/>
       <c r="B105" t="s">
         <v>263</v>
       </c>
@@ -4068,7 +4085,7 @@
       </c>
     </row>
     <row r="106" spans="1:9">
-      <c r="A106" s="11"/>
+      <c r="A106" s="13"/>
       <c r="B106" t="s">
         <v>273</v>
       </c>
@@ -4092,7 +4109,7 @@
       </c>
     </row>
     <row r="107" spans="1:9">
-      <c r="A107" s="11"/>
+      <c r="A107" s="13"/>
       <c r="B107" t="s">
         <v>274</v>
       </c>
@@ -4116,7 +4133,7 @@
       </c>
     </row>
     <row r="108" spans="1:9">
-      <c r="A108" s="11"/>
+      <c r="A108" s="13"/>
       <c r="B108" t="s">
         <v>275</v>
       </c>
@@ -4140,7 +4157,7 @@
       </c>
     </row>
     <row r="109" spans="1:9">
-      <c r="A109" s="11"/>
+      <c r="A109" s="13"/>
       <c r="B109" t="s">
         <v>276</v>
       </c>
@@ -4164,7 +4181,7 @@
       </c>
     </row>
     <row r="110" spans="1:9">
-      <c r="A110" s="11"/>
+      <c r="A110" s="13"/>
       <c r="B110" t="s">
         <v>277</v>
       </c>
@@ -4188,7 +4205,7 @@
       </c>
     </row>
     <row r="111" spans="1:9">
-      <c r="A111" s="11"/>
+      <c r="A111" s="13"/>
       <c r="B111" t="s">
         <v>278</v>
       </c>
@@ -4212,7 +4229,7 @@
       </c>
     </row>
     <row r="112" spans="1:9">
-      <c r="A112" s="11"/>
+      <c r="A112" s="13"/>
       <c r="B112" t="s">
         <v>279</v>
       </c>
@@ -4236,7 +4253,7 @@
       </c>
     </row>
     <row r="113" spans="1:9">
-      <c r="A113" s="11"/>
+      <c r="A113" s="13"/>
       <c r="B113" t="s">
         <v>160</v>
       </c>
@@ -4260,7 +4277,7 @@
       </c>
     </row>
     <row r="114" spans="1:9">
-      <c r="A114" s="11"/>
+      <c r="A114" s="13"/>
       <c r="B114" t="s">
         <v>280</v>
       </c>
@@ -4284,7 +4301,7 @@
       </c>
     </row>
     <row r="115" spans="1:9">
-      <c r="A115" s="11"/>
+      <c r="A115" s="13"/>
       <c r="B115" t="s">
         <v>281</v>
       </c>
@@ -4308,7 +4325,7 @@
       </c>
     </row>
     <row r="116" spans="1:9">
-      <c r="A116" s="11"/>
+      <c r="A116" s="13"/>
       <c r="B116" t="s">
         <v>282</v>
       </c>
@@ -4332,7 +4349,7 @@
       </c>
     </row>
     <row r="117" spans="1:9">
-      <c r="A117" s="11"/>
+      <c r="A117" s="13"/>
       <c r="B117" t="s">
         <v>283</v>
       </c>
@@ -4356,7 +4373,7 @@
       </c>
     </row>
     <row r="118" spans="1:9">
-      <c r="A118" s="11"/>
+      <c r="A118" s="13"/>
       <c r="B118" t="s">
         <v>284</v>
       </c>
@@ -4380,7 +4397,7 @@
       </c>
     </row>
     <row r="119" spans="1:9">
-      <c r="A119" s="11"/>
+      <c r="A119" s="13"/>
       <c r="B119" t="s">
         <v>285</v>
       </c>
@@ -4404,7 +4421,7 @@
       </c>
     </row>
     <row r="120" spans="1:9">
-      <c r="A120" s="11"/>
+      <c r="A120" s="13"/>
       <c r="B120" t="s">
         <v>286</v>
       </c>
@@ -4428,7 +4445,7 @@
       </c>
     </row>
     <row r="121" spans="1:9">
-      <c r="A121" s="11"/>
+      <c r="A121" s="13"/>
       <c r="D121" t="s">
         <v>206</v>
       </c>

</xml_diff>